<commit_message>
restore the template file
</commit_message>
<xml_diff>
--- a/metadata/HealthRICoreP1.xlsx
+++ b/metadata/HealthRICoreP1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manz515245\Documents\HealthRI\excel2rdf\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB82FE58-E0C5-4544-8AEE-9DEBA2AB3939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1AB8BD-035D-4920-994F-68559D5EC353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68415" yWindow="10395" windowWidth="15555" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="69255" yWindow="11235" windowWidth="15555" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DatasetService" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>dct:title</t>
   </si>
@@ -108,22 +108,13 @@
     <t>dash</t>
   </si>
   <si>
-    <t>dcat:endpointURL],</t>
-  </si>
-  <si>
-    <t>sh:property/[</t>
-  </si>
-  <si>
-    <t>dct:title],</t>
-  </si>
-  <si>
-    <t>dcat:endpointDescription],</t>
-  </si>
-  <si>
-    <t>dcat:servesDataset],</t>
-  </si>
-  <si>
-    <t>/[</t>
+    <t>dcat:endpointURL</t>
+  </si>
+  <si>
+    <t>dcat:endpointDescription</t>
+  </si>
+  <si>
+    <t>dcat:servesDataset</t>
   </si>
 </sst>
 </file>
@@ -532,7 +523,7 @@
   <dimension ref="A1:AB17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -659,7 +650,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
@@ -683,10 +674,10 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
@@ -705,10 +696,10 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>6</v>
@@ -727,10 +718,10 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>6</v>

</xml_diff>